<commit_message>
added ability to specify double header for any input. Also fixed button enablement issue
</commit_message>
<xml_diff>
--- a/fixtures/input/faclist.xlsx
+++ b/fixtures/input/faclist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbaker\Documents\HEM4Python\Version1.0\sample files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49B92FD-B8BE-4879-BD67-8C443ADA9346}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7665" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="7668" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>FacilityID</t>
   </si>
@@ -105,6 +106,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Extra header</t>
+  </si>
+  <si>
+    <t>Input category</t>
   </si>
 </sst>
 </file>
@@ -466,136 +473,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDF97E-B161-4714-9981-9B6FC4EE0D5E}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Y2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3">
         <v>3000</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3">
         <v>30</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L3" s="3">
         <v>1.2</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="3" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed user receptors only file to csv and updated tests and test fixtures
</commit_message>
<xml_diff>
--- a/fixtures/input/faclist.xlsx
+++ b/fixtures/input/faclist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49B92FD-B8BE-4879-BD67-8C443ADA9346}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C6D396-7088-41D8-8FBA-02E282F51940}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="7668" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
+    <workbookView xWindow="1260" yWindow="588" windowWidth="20640" windowHeight="11772" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDF97E-B161-4714-9981-9B6FC4EE0D5E}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
corrected math bug in inbox fct of facilityPrep that caused sqrt of neg to be taken
</commit_message>
<xml_diff>
--- a/fixtures/input/faclist.xlsx
+++ b/fixtures/input/faclist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\com\sca\hem4\fixtures\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E8AB39-ECE8-428B-AB42-BFDC272C0218}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF39C8D-76B2-4062-8C85-2CCDB3708E69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>FacilityID</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve">acute  </t>
+  </si>
+  <si>
+    <t>hivalu</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -192,30 +195,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDF97E-B161-4714-9981-9B6FC4EE0D5E}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,44 +603,46 @@
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="8" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="7" t="s">
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="13"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,121 +652,128 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="V2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="3">
+      <c r="E3" s="2"/>
+      <c r="F3" s="3">
         <v>3000</v>
       </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="3">
+      <c r="H3" s="2"/>
+      <c r="I3" s="3">
         <v>30</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3">
         <v>1.2</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="N3" s="3"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:S1"/>
-    <mergeCell ref="T1:Y1"/>
+  <mergeCells count="5">
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="O1:U1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
temporary stop of temporal
</commit_message>
<xml_diff>
--- a/fixtures/input/faclist.xlsx
+++ b/fixtures/input/faclist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\fixtures\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM4\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF39C8D-76B2-4062-8C85-2CCDB3708E69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80022B67-6FAB-4193-9420-00D55A63DB0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
+    <workbookView xWindow="408" yWindow="3588" windowWidth="22788" windowHeight="4716" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>FacilityID</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>hivalu</t>
+  </si>
+  <si>
+    <t>pooping</t>
+  </si>
+  <si>
+    <t>peeing</t>
+  </si>
+  <si>
+    <t>emiss_var</t>
   </si>
 </sst>
 </file>
@@ -253,6 +262,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -265,16 +283,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDF97E-B161-4714-9981-9B6FC4EE0D5E}">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,46 +612,46 @@
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="10" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="7" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="10" t="s">
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="13"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="6"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,56 +682,65 @@
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="AC2" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -739,31 +757,33 @@
         <v>30</v>
       </c>
       <c r="J3" s="3"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3">
         <v>1.2</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="P3" s="3"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
implemented annual/period options in faclist for met data
</commit_message>
<xml_diff>
--- a/fixtures/input/faclist.xlsx
+++ b/fixtures/input/faclist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\fixtures\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM4\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EBD9AD-3147-4ECD-8ACA-5DAAB7DCE5C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA760FE-2534-4D9C-B62E-496C7B7419A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
+    <workbookView xWindow="528" yWindow="168" windowWidth="22512" windowHeight="12156" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>FacilityID</t>
   </si>
@@ -171,13 +171,31 @@
   </si>
   <si>
     <t>emiss_var</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>period_start</t>
+  </si>
+  <si>
+    <t>period_end</t>
+  </si>
+  <si>
+    <t>2016,02,11,12</t>
+  </si>
+  <si>
+    <t>2016,06,30,1</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,12 +222,6 @@
       <name val="MS Sans Serif"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -319,32 +331,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -697,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDF97E-B161-4714-9981-9B6FC4EE0D5E}">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,31 +721,33 @@
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="11" max="11" width="14.77734375" customWidth="1"/>
     <col min="12" max="12" width="12.77734375" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="6" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="11"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="13"/>
       <c r="Q1" s="8" t="s">
         <v>29</v>
       </c>
@@ -742,16 +757,16 @@
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
-      <c r="X1" s="16" t="s">
+      <c r="X1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,10 +797,10 @@
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -836,11 +851,20 @@
       <c r="AB2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AC2" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="AD2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -884,6 +908,15 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
+      <c r="AD3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Updated fixture outputs and faclist input - phase is gone
</commit_message>
<xml_diff>
--- a/fixtures/input/faclist.xlsx
+++ b/fixtures/input/faclist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM4\fixtures\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA760FE-2534-4D9C-B62E-496C7B7419A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F501E90-35A0-47D8-A8D5-8F980B21E947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="528" yWindow="168" windowWidth="22512" windowHeight="12156" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 If this field is left blank, HEM4 will automatically place 13 polar rings /circles by default.</t>
       </text>
     </comment>
-    <comment ref="AC2" authorId="2" shapeId="0" xr:uid="{E2E4CD11-6C69-4415-A625-E5B61AFFF5EB}">
+    <comment ref="AB2" authorId="2" shapeId="0" xr:uid="{E2E4CD11-6C69-4415-A625-E5B61AFFF5EB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>FacilityID</t>
   </si>
@@ -107,9 +107,6 @@
     <t>depl</t>
   </si>
   <si>
-    <t>phase</t>
-  </si>
-  <si>
     <t>pdep</t>
   </si>
   <si>
@@ -180,15 +177,6 @@
   </si>
   <si>
     <t>period_end</t>
-  </si>
-  <si>
-    <t>2016,02,11,12</t>
-  </si>
-  <si>
-    <t>2016,06,30,1</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -237,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -312,18 +300,7 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -331,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -368,9 +345,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -702,7 +676,7 @@
     <text>Ring distances: The user may override HEM4's placement of polar rings ("circles") by specifying a list of distances in this field. Enter a comma separated list that contains at least 3 values representing the distance in meters for the polar ring from the facility center. The distances entered must be &gt; 0 and &lt;= 50000 meters, and the values must be increasing (100,500,1000,5000,10000,50000).
 If this field is left blank, HEM4 will automatically place 13 polar rings /circles by default.</text>
   </threadedComment>
-  <threadedComment ref="AC2" dT="2020-01-30T16:23:55.42" personId="{DF7D7E38-320F-4F86-A82B-634F8D6B1C81}" id="{E2E4CD11-6C69-4415-A625-E5B61AFFF5EB}">
+  <threadedComment ref="AB2" dT="2020-01-30T16:23:55.42" personId="{DF7D7E38-320F-4F86-A82B-634F8D6B1C81}" id="{E2E4CD11-6C69-4415-A625-E5B61AFFF5EB}">
     <text>Emissions Variations: This field allows the application of variations to the emission inputs from specific sources and facilities by different user-supplied time scales (e.g., by season, month, hour of day, day of week), or by different wind speeds (6 ranges). Enter a "Y" in this column for a given facility (or facilities) if you want to vary the emissions for one or more sources at that facility (or facilities). Note: HEM4 will prompt you for an emissions variation file if you entered "Y" for one or more facilities, and that file must contain variation factors for at least one source at each facility marked with a "Y".</text>
   </threadedComment>
 </ThreadedComments>
@@ -710,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDF97E-B161-4714-9981-9B6FC4EE0D5E}">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,19 +695,19 @@
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="11" max="11" width="14.77734375" customWidth="1"/>
     <col min="12" max="12" width="12.77734375" customWidth="1"/>
-    <col min="31" max="31" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
       <c r="E1" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
@@ -743,30 +717,32 @@
       <c r="K1" s="15"/>
       <c r="L1" s="16"/>
       <c r="M1" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
       <c r="P1" s="13"/>
       <c r="Q1" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
       <c r="T1" s="8"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
+      <c r="W1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +753,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
@@ -798,13 +774,13 @@
         <v>11</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>8</v>
@@ -813,7 +789,7 @@
         <v>10</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>12</v>
@@ -833,11 +809,11 @@
       <c r="V2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>19</v>
@@ -846,12 +822,12 @@
         <v>20</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" s="7" t="s">
         <v>35</v>
       </c>
       <c r="AD2" s="7" t="s">
@@ -860,13 +836,10 @@
       <c r="AE2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="7" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -884,7 +857,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3">
@@ -898,33 +871,23 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="X3" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="Y3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="Q1:V1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="E1:L1"/>
-    <mergeCell ref="X1:AC1"/>
+    <mergeCell ref="W1:AE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed label highlight issue
</commit_message>
<xml_diff>
--- a/fixtures/input/faclist.xlsx
+++ b/fixtures/input/faclist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\fixtures\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Lindsey\OneDrive - SC&amp;A, Inc\Documents\HEM4\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F501E90-35A0-47D8-A8D5-8F980B21E947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1757E08A-8C39-403D-B43D-898C530DC602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
+    <workbookView xWindow="600" yWindow="1800" windowWidth="25965" windowHeight="13800" xr2:uid="{6DACADE6-3D82-4463-B55D-EC7754581E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 If this field is left blank, HEM4 will automatically place 13 polar rings /circles by default.</t>
       </text>
     </comment>
-    <comment ref="AB2" authorId="2" shapeId="0" xr:uid="{E2E4CD11-6C69-4415-A625-E5B61AFFF5EB}">
+    <comment ref="AA2" authorId="2" shapeId="0" xr:uid="{E2E4CD11-6C69-4415-A625-E5B61AFFF5EB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>FacilityID</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>vdepl</t>
-  </si>
-  <si>
-    <t>All_rcpts</t>
   </si>
   <si>
     <t>user_rcpt</t>
@@ -676,7 +673,7 @@
     <text>Ring distances: The user may override HEM4's placement of polar rings ("circles") by specifying a list of distances in this field. Enter a comma separated list that contains at least 3 values representing the distance in meters for the polar ring from the facility center. The distances entered must be &gt; 0 and &lt;= 50000 meters, and the values must be increasing (100,500,1000,5000,10000,50000).
 If this field is left blank, HEM4 will automatically place 13 polar rings /circles by default.</text>
   </threadedComment>
-  <threadedComment ref="AB2" dT="2020-01-30T16:23:55.42" personId="{DF7D7E38-320F-4F86-A82B-634F8D6B1C81}" id="{E2E4CD11-6C69-4415-A625-E5B61AFFF5EB}">
+  <threadedComment ref="AA2" dT="2020-01-30T16:23:55.42" personId="{DF7D7E38-320F-4F86-A82B-634F8D6B1C81}" id="{E2E4CD11-6C69-4415-A625-E5B61AFFF5EB}">
     <text>Emissions Variations: This field allows the application of variations to the emission inputs from specific sources and facilities by different user-supplied time scales (e.g., by season, month, hour of day, day of week), or by different wind speeds (6 ranges). Enter a "Y" in this column for a given facility (or facilities) if you want to vary the emissions for one or more sources at that facility (or facilities). Note: HEM4 will prompt you for an emissions variation file if you entered "Y" for one or more facilities, and that file must contain variation factors for at least one source at each facility marked with a "Y".</text>
   </threadedComment>
 </ThreadedComments>
@@ -684,30 +681,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDF97E-B161-4714-9981-9B6FC4EE0D5E}">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X1:X1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" customWidth="1"/>
-    <col min="30" max="30" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
       <c r="E1" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
@@ -717,13 +714,13 @@
       <c r="K1" s="15"/>
       <c r="L1" s="16"/>
       <c r="M1" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
       <c r="P1" s="13"/>
       <c r="Q1" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
@@ -731,7 +728,7 @@
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
       <c r="W1" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X1" s="9"/>
       <c r="Y1" s="9"/>
@@ -740,9 +737,8 @@
       <c r="AB1" s="9"/>
       <c r="AC1" s="9"/>
       <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +749,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
@@ -774,13 +770,13 @@
         <v>11</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>8</v>
@@ -789,7 +785,7 @@
         <v>10</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>12</v>
@@ -819,12 +815,12 @@
         <v>19</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB2" s="7" t="s">
         <v>34</v>
       </c>
       <c r="AC2" s="7" t="s">
@@ -833,13 +829,10 @@
       <c r="AD2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="7" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -857,7 +850,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3">
@@ -872,14 +865,11 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -887,7 +877,7 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="E1:L1"/>
-    <mergeCell ref="W1:AE1"/>
+    <mergeCell ref="W1:AD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>